<commit_message>
CATGrammar SimpleStatemnent completed (still some cases)
</commit_message>
<xml_diff>
--- a/Temp_folder/Caso Kola Real.xlsx
+++ b/Temp_folder/Caso Kola Real.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dave_PersonalCarpet\code\2020_01\Temp_folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dave\code\2020_01\Temp_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10320" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10320" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="EFE" sheetId="1" r:id="rId1"/>
     <sheet name="EFI" sheetId="2" r:id="rId2"/>
+    <sheet name="FODA Cruzado" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="91">
   <si>
     <t xml:space="preserve">Oportunidades </t>
   </si>
@@ -57,21 +58,6 @@
     <t>O8</t>
   </si>
   <si>
-    <t>O9</t>
-  </si>
-  <si>
-    <t>O10</t>
-  </si>
-  <si>
-    <t>O11</t>
-  </si>
-  <si>
-    <t>O12</t>
-  </si>
-  <si>
-    <t>O13</t>
-  </si>
-  <si>
     <t>Amenazas</t>
   </si>
   <si>
@@ -102,24 +88,12 @@
     <t>Caso Kola Real</t>
   </si>
   <si>
-    <t>(O) En ayacucho, en la epoca del terrorismo, los proveedores externo tenían dificultades para distribuir sus productos.</t>
-  </si>
-  <si>
     <t>Matriz EFI - Evaluación de Factores Internos</t>
   </si>
   <si>
     <t>Uno de sus fundadores tenía experiencia en la distribución del producto.</t>
   </si>
   <si>
-    <t>(O) Durante un tiempo se intento esparcir mala fama a la empresa por la epidemia del Cólera.</t>
-  </si>
-  <si>
-    <t>(O) Durante sus inicios, un anormalmente largo fenómeno del Niño favoreció sus ventas y le permitió reinvertir.</t>
-  </si>
-  <si>
-    <t>(O) En Puebla se disponde de un terreno geográficamente estrátegico, de bajo costo y con un buen aprovisionamiento de agua.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fortalezas </t>
   </si>
   <si>
@@ -132,24 +106,12 @@
     <t>Con el crecimiento del mercado, aumenta el número de competidores.</t>
   </si>
   <si>
-    <t>Trato directo con los pequeños comerciates ofreciendo mejores condiciones que la competencia (Estrategia de concentración).</t>
-  </si>
-  <si>
     <t>El propio crecimiento de la empreso impulsó el desarrollo del mercado hasta en un 300%. (Masificación en el consumo de gaseosas)</t>
   </si>
   <si>
-    <t>Cambios en el manejo de la gestión sumamente rápidos.</t>
-  </si>
-  <si>
     <t>No pasaron por el proceso de descubrir un mercado, pues ellos provienen de ahí.</t>
   </si>
   <si>
-    <t>(O) En Venezuela solo el 3% del mercado se realiza en envases PET</t>
-  </si>
-  <si>
-    <t>(O) En Perú, el beneficio tributario decretado por Fujimori para con las empresas en la Amazonía.</t>
-  </si>
-  <si>
     <t>Ser una marca propia les evita pagar el 18% por concepto de franquicia.</t>
   </si>
   <si>
@@ -159,17 +121,214 @@
     <t>Gastos administrativos muy reducidos.</t>
   </si>
   <si>
-    <t>Compromiso e involucramiento del personal.</t>
-  </si>
-  <si>
     <t>Estrategia netamente enfocada en la calidad del producto en donde se combinan costo junto a la ampliación del mercado (Liderazgo en razones de costo).</t>
+  </si>
+  <si>
+    <t>La administración familiar de la empresa no admite profesionales  independientes haciendo de la misma una Pyme a gran escala.</t>
+  </si>
+  <si>
+    <t>Posee una organización muy artesanal, poco estructurada y basada solo en el olfato.</t>
+  </si>
+  <si>
+    <t>Trato directo con los pequeños comerciantes ofreciendo mejores condiciones que la competencia (Estrategia de concentración).</t>
+  </si>
+  <si>
+    <t>Uso de tecnologías robóticas con asociados de Alemania y Francia.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">La experiencia del mercado Mexicano y su elevado </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>expertise</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> elevan los estándares del producto</t>
+    </r>
+  </si>
+  <si>
+    <t>Cambios en el manejo de la gestión sumamente rápidos. Políticas enfocadas a la no burocratización pero si a la rapidez de las acciones.</t>
+  </si>
+  <si>
+    <t>Compromiso e involucramiento del personal reflejados en su filosofía de trabajo.</t>
+  </si>
+  <si>
+    <t>Se sacrifican ciertos atributos de atributos que ofrecen los productos de los todistas.</t>
+  </si>
+  <si>
+    <t>(P) Durante un tiempo se intento esparcir mala fama a la empresa por la epidemia del Cólera.</t>
+  </si>
+  <si>
+    <t>(P) En ayacucho, en la epoca del terrorismo, los proveedores externo tenían dificultades para distribuir sus productos.</t>
+  </si>
+  <si>
+    <t>(P) Durante sus inicios, un anormalmente largo fenómeno del Niño favoreció sus ventas y le permitió reinvertir.</t>
+  </si>
+  <si>
+    <t>(P) En Perú, el beneficio tributario decretado por Fujimori para con las empresas en la Amazonía.</t>
+  </si>
+  <si>
+    <t>(P) Actualment, en Puebla se disponde de un terreno geográficamente estrátegico, de bajo costo y con un buen aprovisionamiento de agua.</t>
+  </si>
+  <si>
+    <t>(P) En Venezuela solo el 3% del mercado se realiza en envases PET</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>Oportunidades</t>
+  </si>
+  <si>
+    <t>Estrategias FO</t>
+  </si>
+  <si>
+    <t>ESTRATEGIAS DO</t>
+  </si>
+  <si>
+    <t>Estrategias FA</t>
+  </si>
+  <si>
+    <t>Estrategias DA</t>
+  </si>
+  <si>
+    <t>FO1</t>
+  </si>
+  <si>
+    <t>FO2</t>
+  </si>
+  <si>
+    <t>FO3</t>
+  </si>
+  <si>
+    <t>FO4</t>
+  </si>
+  <si>
+    <t>FO5</t>
+  </si>
+  <si>
+    <t>FO6</t>
+  </si>
+  <si>
+    <t>FO7</t>
+  </si>
+  <si>
+    <t>FO8</t>
+  </si>
+  <si>
+    <t>FA1</t>
+  </si>
+  <si>
+    <t>FA2</t>
+  </si>
+  <si>
+    <t>FA3</t>
+  </si>
+  <si>
+    <t>DO1</t>
+  </si>
+  <si>
+    <t>DO2</t>
+  </si>
+  <si>
+    <t>DO3</t>
+  </si>
+  <si>
+    <t>DO4</t>
+  </si>
+  <si>
+    <t>DO5</t>
+  </si>
+  <si>
+    <t>DO6</t>
+  </si>
+  <si>
+    <t>DO7</t>
+  </si>
+  <si>
+    <t>DO8</t>
+  </si>
+  <si>
+    <t>DA1</t>
+  </si>
+  <si>
+    <t>DA2</t>
+  </si>
+  <si>
+    <t>DA3</t>
+  </si>
+  <si>
+    <t>Aprovechar la ausencia de proveedores externos asegurándose un nicho en función a las perpectivas de su propia comunidad (F1, F2, O1).</t>
+  </si>
+  <si>
+    <t>Aperturar nuevas plantas de producción de manera acelerada y en función al potencial de desarrollo en un mercado (F5,  F8, F9, O2, ).</t>
+  </si>
+  <si>
+    <t>Aperturar nuevas plantas de producción de manera acelerada y en función al potencial de desarrollo en un mercado (F5,  F8, F9, O2, O6, O8).</t>
+  </si>
+  <si>
+    <t>Aperturar nuevas plantas de producción de manera acelerada y aprovechando las ventajas políticas, geográficas y del mercado según el lugar (F5, F8, F9, O3, O4, O5).</t>
+  </si>
+  <si>
+    <t>El propio crecimiento de la empreso puede impulsar el desarrollo del mercado hasta en un 300%. (Masificación en el consumo de gaseosas)</t>
+  </si>
+  <si>
+    <t>Respaldar la calidad de su producto  a la vez que se ofrece mejores precios que la competencia para con los segmentos más pobres del mercado asegurándose un nicho (F3, O7, O8).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,16 +344,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -202,20 +375,199 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -497,23 +849,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B27"/>
+  <dimension ref="A2:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="122.140625" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="140.28515625" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -530,7 +883,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -538,7 +891,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -546,7 +899,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -554,7 +907,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -562,7 +915,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -570,7 +923,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -578,7 +931,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -586,11 +939,11 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -598,16 +951,25 @@
       <c r="A15" t="s">
         <v>11</v>
       </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -615,7 +977,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
@@ -623,46 +985,15 @@
       <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="B20" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
-      <c r="B21" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -676,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B27"/>
+  <dimension ref="A2:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,29 +1020,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
@@ -719,23 +1053,23 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
@@ -743,99 +1077,63 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
+      <c r="B15" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>23</v>
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -844,4 +1142,351 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E2:J25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="57.7109375" customWidth="1"/>
+    <col min="8" max="8" width="63.140625" customWidth="1"/>
+    <col min="10" max="10" width="48.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="4"/>
+      <c r="H3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="G4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="G5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="5:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="G7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="G8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="G9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="G10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="G11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="5:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="11"/>
+      <c r="F13" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14" s="14"/>
+    </row>
+    <row r="15" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E15" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E19" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="5:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="5:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="11"/>
+      <c r="F22" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="17"/>
+      <c r="H22" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I22" s="17"/>
+      <c r="J22" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="J23" s="14"/>
+    </row>
+    <row r="24" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E24" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E25" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J25" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>